<commit_message>
week 5 - exam results updated
</commit_message>
<xml_diff>
--- a/exam_results/Participants.xlsx
+++ b/exam_results/Participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E7BA8B-F32A-0349-BD74-E8BFF81578FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17866FC-863C-5B42-B629-64CA92F90922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="357">
   <si>
     <t>Ad</t>
   </si>
@@ -1085,6 +1085,12 @@
   </si>
   <si>
     <t>Hmw2</t>
+  </si>
+  <si>
+    <t>*****</t>
+  </si>
+  <si>
+    <t>****</t>
   </si>
 </sst>
 </file>
@@ -1441,9 +1447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" activeCellId="1" sqref="C64 C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1529,6 +1535,9 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1601,6 +1610,9 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
+      <c r="D12">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1655,7 +1667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1683,7 +1695,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1711,7 +1723,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1722,7 +1734,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1733,7 +1745,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1744,7 +1756,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1755,7 +1767,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1765,8 +1777,11 @@
       <c r="C25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1780,7 +1795,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1794,7 +1809,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1808,7 +1823,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1819,7 +1834,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -1830,7 +1845,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -1844,7 +1859,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1907,6 +1922,9 @@
       <c r="C36" t="s">
         <v>106</v>
       </c>
+      <c r="D36">
+        <v>75</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1943,6 +1961,9 @@
       <c r="C39" t="s">
         <v>115</v>
       </c>
+      <c r="D39">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -2004,6 +2025,9 @@
       <c r="C44" t="s">
         <v>130</v>
       </c>
+      <c r="D44">
+        <v>90</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2154,6 +2178,9 @@
       <c r="C56" t="s">
         <v>166</v>
       </c>
+      <c r="D56">
+        <v>70</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -2240,6 +2267,9 @@
       <c r="C63" t="s">
         <v>187</v>
       </c>
+      <c r="D63">
+        <v>100</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
@@ -2301,6 +2331,9 @@
       <c r="C68" t="s">
         <v>202</v>
       </c>
+      <c r="D68">
+        <v>85</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -2455,7 +2488,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>239</v>
       </c>
@@ -2469,7 +2502,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>242</v>
       </c>
@@ -2483,7 +2516,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>245</v>
       </c>
@@ -2497,7 +2530,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>248</v>
       </c>
@@ -2508,7 +2541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>251</v>
       </c>
@@ -2518,8 +2551,11 @@
       <c r="C85" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>254</v>
       </c>
@@ -2529,8 +2565,11 @@
       <c r="C86" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>257</v>
       </c>
@@ -2541,7 +2580,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>260</v>
       </c>
@@ -2552,7 +2591,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>263</v>
       </c>
@@ -2563,7 +2602,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>266</v>
       </c>
@@ -2577,7 +2616,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>269</v>
       </c>
@@ -2588,7 +2627,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>272</v>
       </c>
@@ -2599,7 +2638,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>275</v>
       </c>
@@ -2613,7 +2652,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -2627,7 +2666,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>281</v>
       </c>
@@ -2641,7 +2680,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>284</v>
       </c>

</xml_diff>